<commit_message>
add x y z for IObject.xlsx
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/IObject.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/IObject.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView windowWidth="20730" windowHeight="9172"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>Id</t>
   </si>
@@ -47,6 +34,15 @@
     <t>ConfigID</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -56,6 +52,9 @@
     <t>int</t>
   </si>
   <si>
+    <t>float</t>
+  </si>
+  <si>
     <t>Public</t>
   </si>
   <si>
@@ -71,21 +70,26 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Upload</t>
+  </si>
+  <si>
     <t>Desc</t>
   </si>
   <si>
     <t>0全局广播</t>
-  </si>
-  <si>
-    <t>Upload</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -107,12 +111,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +281,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -256,9 +592,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -306,19 +884,58 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -645,27 +1262,28 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="1" max="2" width="10.4513274336283" customWidth="1"/>
+    <col min="3" max="4" width="8.45132743362832" customWidth="1"/>
+    <col min="5" max="5" width="9.45132743362832" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -684,30 +1302,48 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="1" spans="1:9">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="2" customFormat="1" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" s="9" t="b">
         <v>0</v>
@@ -724,10 +1360,19 @@
       <c r="F3" s="10" t="b">
         <v>0</v>
       </c>
+      <c r="G3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" spans="1:9">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>1</v>
@@ -744,10 +1389,19 @@
       <c r="F4" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="G4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" s="2" customFormat="1" spans="1:9">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" s="9" t="b">
         <v>0</v>
@@ -764,10 +1418,19 @@
       <c r="F5" s="10" t="b">
         <v>0</v>
       </c>
+      <c r="G5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" spans="1:9">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9" t="b">
         <v>0</v>
@@ -784,10 +1447,19 @@
       <c r="F6" s="10" t="b">
         <v>0</v>
       </c>
+      <c r="G6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="3" customFormat="1" spans="1:9">
       <c r="A7" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -804,10 +1476,19 @@
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="3" customFormat="1" spans="1:9">
       <c r="A8" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -824,28 +1505,36 @@
       <c r="F8" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" s="4" customFormat="1" ht="14.25" spans="1:6">
       <c r="A9" s="12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9" s="13"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F1048576 F2:F6 B7:J8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 H3 I3 G4 H4 I4 G5 H5 I5 G6 H6 I6 B7:F7 G7 H7 I7 J7 B8:F8 G8 H8 I8 J8 F2:F6 F9:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>